<commit_message>
data for modeling the motors
</commit_message>
<xml_diff>
--- a/thurt_RMP_Voltage_table.xlsx
+++ b/thurt_RMP_Voltage_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c309fd16b2100de/Documents/git/magic_juggle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2FCE8D89-90F4-451C-BE02-4C545FEEE93F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{2FCE8D89-90F4-451C-BE02-4C545FEEE93F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{565F3256-0147-47CA-BF67-FE1E71DFB262}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{7B91EFB9-1645-4214-BEEC-AF5D28490A57}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Amps</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Average RPM</t>
+  </si>
+  <si>
+    <t>Thrust (N)</t>
   </si>
 </sst>
 </file>
@@ -189,27 +192,25 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
+              <c:f>Sheet1!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Average RPM</c:v>
+                  <c:v>Thrust (N)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -229,64 +230,58 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.24052108899722624"/>
+                  <c:y val="8.8150201854873753E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pt-BR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10.9</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13.9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>17.3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>24.4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>28.6</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>32.799999999999997</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>37.299999999999997</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>41.7</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>51.9</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>57.9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$E$2:$E$17</c:f>
               <c:numCache>
@@ -342,11 +337,68 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5679999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.7039999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.7420000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.10682</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.13622000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.16954</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.20579999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.23911999999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.28028000000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.32143999999999995</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.36553999999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.40866000000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.45079999999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.50861999999999996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.56741999999999992</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F4DB-40C0-8FFD-69B94BF07770}"/>
+              <c16:uniqueId val="{00000000-A1D8-4F3A-B932-043F281435B2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -358,11 +410,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2012105071"/>
-        <c:axId val="1959889327"/>
+        <c:axId val="307400687"/>
+        <c:axId val="127286815"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2012105071"/>
+        <c:axId val="307400687"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -419,12 +471,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1959889327"/>
+        <c:crossAx val="127286815"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1959889327"/>
+        <c:axId val="127286815"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -481,428 +533,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2012105071"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="pt-BR"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="7.4914260717410336E-2"/>
-          <c:y val="0.14393518518518519"/>
-          <c:w val="0.87119685039370076"/>
-          <c:h val="0.72088764946048411"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Thrust (g)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$E$2:$E$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4485</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7570</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9374</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10885</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>12277</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>13522</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>14691</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>15924</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>17174</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>18179</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>19397</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>20539</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>21692</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>22598</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>23882</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$F$2:$F$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10.9</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13.9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>17.3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>24.4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>28.6</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>32.799999999999997</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>37.299999999999997</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>41.7</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>51.9</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>57.9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-38A6-4DFF-88FE-11A51A39ABAD}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="2005477967"/>
-        <c:axId val="1959879759"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="2005477967"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1959879759"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="1959879759"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2005477967"/>
+        <c:crossAx val="307400687"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -998,563 +629,7 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2075,22 +1150,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC417A80-2CAD-48E6-A17E-D56E148F7FFA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F04919B4-103F-4D81-8A38-DB69434C624F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2103,42 +1178,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>295274</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7B376A7-BCF7-4519-BBD1-6B48AD28F8E6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2444,15 +1483,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63B3E12F-AD81-4521-8E19-0857CBB59AC2}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="T29" sqref="T29"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E1" activeCellId="1" sqref="G1:G17 E1:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2471,8 +1510,11 @@
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0.24</v>
       </c>
@@ -2491,8 +1533,12 @@
       <c r="F2" s="1">
         <v>0</v>
       </c>
+      <c r="G2">
+        <f>F2*0.0098</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>0.37</v>
       </c>
@@ -2511,8 +1557,12 @@
       <c r="F3" s="1">
         <v>1.6</v>
       </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G17" si="0">F3*0.0098</f>
+        <v>1.5679999999999999E-2</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>0.56000000000000005</v>
       </c>
@@ -2531,8 +1581,12 @@
       <c r="F4" s="1">
         <v>4.8</v>
       </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>4.7039999999999998E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>0.75</v>
       </c>
@@ -2551,8 +1605,12 @@
       <c r="F5" s="1">
         <v>7.9</v>
       </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>7.7420000000000003E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>0.94</v>
       </c>
@@ -2571,8 +1629,12 @@
       <c r="F6" s="1">
         <v>10.9</v>
       </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>0.10682</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1.1499999999999999</v>
       </c>
@@ -2591,8 +1653,12 @@
       <c r="F7" s="1">
         <v>13.9</v>
       </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0.13622000000000001</v>
+      </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1.37</v>
       </c>
@@ -2611,8 +1677,12 @@
       <c r="F8" s="1">
         <v>17.3</v>
       </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>0.16954</v>
+      </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>1.59</v>
       </c>
@@ -2631,8 +1701,12 @@
       <c r="F9" s="1">
         <v>21</v>
       </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>0.20579999999999998</v>
+      </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>1.83</v>
       </c>
@@ -2651,8 +1725,12 @@
       <c r="F10" s="1">
         <v>24.4</v>
       </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>0.23911999999999997</v>
+      </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>2.11</v>
       </c>
@@ -2671,8 +1749,12 @@
       <c r="F11" s="1">
         <v>28.6</v>
       </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>0.28028000000000003</v>
+      </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>2.39</v>
       </c>
@@ -2691,8 +1773,12 @@
       <c r="F12" s="1">
         <v>32.799999999999997</v>
       </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>0.32143999999999995</v>
+      </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>2.71</v>
       </c>
@@ -2711,8 +1797,12 @@
       <c r="F13" s="1">
         <v>37.299999999999997</v>
       </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>0.36553999999999998</v>
+      </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>3.06</v>
       </c>
@@ -2731,8 +1821,12 @@
       <c r="F14" s="1">
         <v>41.7</v>
       </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>0.40866000000000002</v>
+      </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>3.46</v>
       </c>
@@ -2751,8 +1845,12 @@
       <c r="F15" s="1">
         <v>46</v>
       </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>0.45079999999999998</v>
+      </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>3.88</v>
       </c>
@@ -2771,8 +1869,12 @@
       <c r="F16" s="1">
         <v>51.9</v>
       </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>0.50861999999999996</v>
+      </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>4.4400000000000004</v>
       </c>
@@ -2790,6 +1892,10 @@
       </c>
       <c r="F17" s="2">
         <v>57.9</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>0.56741999999999992</v>
       </c>
     </row>
   </sheetData>

</xml_diff>